<commit_message>
Updated MCH102 to MCH251
</commit_message>
<xml_diff>
--- a/Historical Papers/Collections/MCH105.xlsx
+++ b/Historical Papers/Collections/MCH105.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="132" yWindow="504" windowWidth="18876" windowHeight="9732"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
   <si>
     <t>identifier</t>
   </si>
@@ -35,29 +38,212 @@
   </si>
   <si>
     <t>file_path</t>
+  </si>
+  <si>
+    <t>MCH105-1</t>
+  </si>
+  <si>
+    <t>NSC</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>1 Box</t>
+  </si>
+  <si>
+    <t>LOCATION: 20N | GRAP COUNT NUMER: NONE</t>
+  </si>
+  <si>
+    <t>MCH105-2</t>
+  </si>
+  <si>
+    <t>NATIONAL OLYMPICS</t>
+  </si>
+  <si>
+    <t>MCH105-3</t>
+  </si>
+  <si>
+    <t>NSC REPORTS</t>
+  </si>
+  <si>
+    <t>LOCATION: 20O | GRAP COUNT NUMER: NONE</t>
+  </si>
+  <si>
+    <t>MCH105-4</t>
+  </si>
+  <si>
+    <t>OLYMPIC 2004</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>MCH105-5</t>
+  </si>
+  <si>
+    <t>MCH105-6</t>
+  </si>
+  <si>
+    <t>MCH105-7</t>
+  </si>
+  <si>
+    <t>CAPE TOWN 2004 OLYMPIC BID</t>
+  </si>
+  <si>
+    <t>MCH105-8</t>
+  </si>
+  <si>
+    <t>NSC DOCUMENTS (SPORT)</t>
+  </si>
+  <si>
+    <t>MCH105-9</t>
+  </si>
+  <si>
+    <t>SPORT, STICKERS, PUBLICATIONS, CAPE TOWN OLYMPIC BID</t>
+  </si>
+  <si>
+    <t>MCH105-10</t>
+  </si>
+  <si>
+    <t>NATIONAL SPORT COUNCIL</t>
+  </si>
+  <si>
+    <t>MCH105-11</t>
+  </si>
+  <si>
+    <t>MCH105-12</t>
+  </si>
+  <si>
+    <t>SPORT, NSC SPORT SCIENCE INSTITUTE, GREATER CAPE TOWN CAMPAIGN</t>
+  </si>
+  <si>
+    <t>MCH105-13</t>
+  </si>
+  <si>
+    <t>NSC CORRESPONDENCE</t>
+  </si>
+  <si>
+    <t>LOCATION: 20P | GRAP COUNT NUMER: NONE</t>
+  </si>
+  <si>
+    <t>MCH105-14</t>
+  </si>
+  <si>
+    <t>SPORT- DIFFERENT SPORTS CODES, OLYMPIC PRESENTATION</t>
+  </si>
+  <si>
+    <t>MCH105-15</t>
+  </si>
+  <si>
+    <t>SPORTS IN GENERAL NSC</t>
+  </si>
+  <si>
+    <t>MCH105-16</t>
+  </si>
+  <si>
+    <t>MCH105-17</t>
+  </si>
+  <si>
+    <t>SPORT, NSC, GREATER CAPE TOWN , SPORTS COMMISSION</t>
+  </si>
+  <si>
+    <t>MCH105-18</t>
+  </si>
+  <si>
+    <t>DEPT OF SPORT WESTERN CAPE</t>
+  </si>
+  <si>
+    <t>MCH105-19</t>
+  </si>
+  <si>
+    <t>NSC SPORTING CODES</t>
+  </si>
+  <si>
+    <t>MCH105-20</t>
+  </si>
+  <si>
+    <t>GREATER CAPE TOWN COMMISSION 1994</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>MCH105-21</t>
+  </si>
+  <si>
+    <t>OLYMPIC 2004 BID</t>
+  </si>
+  <si>
+    <t>MCH105-22</t>
+  </si>
+  <si>
+    <t>(NOCSA) CAPE TOWN 2004 BID</t>
+  </si>
+  <si>
+    <t>MCH105-23</t>
+  </si>
+  <si>
+    <t>FUNDING</t>
+  </si>
+  <si>
+    <t>LOCATION: 21A | GRAP COUNT NUMER: NONE</t>
+  </si>
+  <si>
+    <t>MCH105-24</t>
+  </si>
+  <si>
+    <t>MCH105-25</t>
+  </si>
+  <si>
+    <t>CTN OLYMPIC BID</t>
+  </si>
+  <si>
+    <t>MCH105-26</t>
+  </si>
+  <si>
+    <t>SPORTING CODES OLYMPICS</t>
+  </si>
+  <si>
+    <t>MCH105-27</t>
+  </si>
+  <si>
+    <t>CAPE TOWN OLYMPIC BID</t>
+  </si>
+  <si>
+    <t>MCH105-28</t>
+  </si>
+  <si>
+    <t>SPORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -65,7 +251,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -75,33 +261,39 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -291,28 +483,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.0"/>
-    <col customWidth="1" min="5" max="5" width="15.13"/>
-    <col customWidth="1" min="6" max="6" width="15.38"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -356,7 +551,547 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>